<commit_message>
fix type on open_source_aib_csr.xlsx
Signed-off-by: huizhan1 <julie.zhang@intel.com>
</commit_message>
<xml_diff>
--- a/docs/open_source_aib_csr.xlsx
+++ b/docs/open_source_aib_csr.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/julie_zhang_intel_com/Documents/Shared Documents/DARPA/open source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OWR\aib_phy_hardware_rev0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="8_{4CD06FE8-E8BE-4447-9F86-000E18B250FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{DD8ABC64-532A-4FC0-B448-1625F7227710}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B92CD8A-E933-458E-B982-F5BE1088BCAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27060" windowHeight="11655" activeTab="1" xr2:uid="{C6002A17-3870-4AD4-B97B-45CCDF04E806}"/>
   </bookViews>
@@ -5723,7 +5723,7 @@
   <dimension ref="A1:H836"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F163" sqref="F162:F163"/>
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8025,7 +8025,7 @@
       <c r="A149" s="35"/>
       <c r="B149" s="35"/>
       <c r="C149" s="40" t="s">
-        <v>297</v>
+        <v>487</v>
       </c>
       <c r="D149" s="30" t="s">
         <v>298</v>
@@ -30902,6 +30902,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D03D0EE2D2295446876114B826DEF78D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="672737267bedf5b9e80c74c088225302">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="bbb4e383-f888-41b5-a796-2bb1d9ab62ae" xmlns:ns4="530af12c-1954-46ad-9c94-ddb07003369d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c0fbb07d547c34ba17ecd0fbb537a2c" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -31121,25 +31139,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5536D9E3-D332-4E90-BF7B-48E6B0DB3F0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="bbb4e383-f888-41b5-a796-2bb1d9ab62ae"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="530af12c-1954-46ad-9c94-ddb07003369d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90F41780-9094-4F4A-BE43-209970D09E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFB09BA0-4BE5-4947-B434-0DF2A857D4E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31157,30 +31183,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90F41780-9094-4F4A-BE43-209970D09E33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5536D9E3-D332-4E90-BF7B-48E6B0DB3F0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="bbb4e383-f888-41b5-a796-2bb1d9ab62ae"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="530af12c-1954-46ad-9c94-ddb07003369d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added v2s configuration page
Signed-off-by: Julie Zhang <julie.zhang@intel.com>
</commit_message>
<xml_diff>
--- a/docs/open_source_aib_csr.xlsx
+++ b/docs/open_source_aib_csr.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OWR\aib_phy_hardware_rev0\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/julie_zhang_intel_com/Documents/Shared Documents/DARPA/open source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B92CD8A-E933-458E-B982-F5BE1088BCAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{10E8AE15-6EF5-410C-B794-3DF6F6DB49DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{3C658EDA-5839-4D92-8EDC-463A4CE5046A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27060" windowHeight="11655" activeTab="1" xr2:uid="{C6002A17-3870-4AD4-B97B-45CCDF04E806}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="23040" windowHeight="12915" activeTab="1" xr2:uid="{C6002A17-3870-4AD4-B97B-45CCDF04E806}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
     <sheet name="usr_csr" sheetId="4" r:id="rId2"/>
     <sheet name="cfg_csr" sheetId="3" r:id="rId3"/>
     <sheet name="dll-dcc fsm port description" sheetId="5" r:id="rId4"/>
+    <sheet name="v2_slave" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_Hlk40449787" localSheetId="4">v2_slave!$F$33</definedName>
     <definedName name="RW_VALIDATION1">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="1284">
   <si>
     <t xml:space="preserve">This spread sheet illustrated register bit setting of one channel c3aibadapt_wrap.v file (Diagram at the left side) </t>
   </si>
@@ -2745,9 +2747,6 @@
   </si>
   <si>
     <t>1'b1    Test mode enable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27:24      </t>
   </si>
   <si>
     <t>csr_reg[51]</t>
@@ -3783,12 +3782,165 @@
   <si>
     <t xml:space="preserve">21     </t>
   </si>
+  <si>
+    <t>4’b0</t>
+  </si>
+  <si>
+    <t>Reserved.</t>
+  </si>
+  <si>
+    <t>1’b0</t>
+  </si>
+  <si>
+    <t>r_rx_double_read:</t>
+  </si>
+  <si>
+    <t>1:receive fifo read 2x width.2x phase comp fifo mode.</t>
+  </si>
+  <si>
+    <t>0: receive fifo read 1x width. 1x phase comp fifo mode.</t>
+  </si>
+  <si>
+    <t>26’b0</t>
+  </si>
+  <si>
+    <t>rxswap_en:(only used in  fifo 2x mode. This bit can not be set to “1” in register mode and fifo 1x mode)</t>
+  </si>
+  <si>
+    <t>1:The upper/lower word(bit[77:39]/bit[38:0])  of the receive data sent to MAC(data_out[77:0], refer to table  3) is swapped. The upper/lower word of the loopback data in loopback path 3(Figure 9) is also swapped in 2x fifo loopback path 3 mode.</t>
+  </si>
+  <si>
+    <t>0: No swapping of data.</t>
+  </si>
+  <si>
+    <t>0x20c</t>
+  </si>
+  <si>
+    <t>25’b0</t>
+  </si>
+  <si>
+    <t>r_rx_lpbk: loop back path 1 enable</t>
+  </si>
+  <si>
+    <t>1: loop back path 1 enable</t>
+  </si>
+  <si>
+    <t>0: loop back path 1 disable</t>
+  </si>
+  <si>
+    <t>6’b0</t>
+  </si>
+  <si>
+    <t>29’b0</t>
+  </si>
+  <si>
+    <t>2’b00</t>
+  </si>
+  <si>
+    <t>rx_fifo_mode:</t>
+  </si>
+  <si>
+    <t>00: receive 1x  fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>01: receive 2x fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>11: receive register mode.</t>
+  </si>
+  <si>
+    <t>rx_wa_en:</t>
+  </si>
+  <si>
+    <t>1: receive word alignment enable. For 2x fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>0: receive word alignment disable. For 1x fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>8’b0</t>
+  </si>
+  <si>
+    <t>tx_wm_en:</t>
+  </si>
+  <si>
+    <t>1: enable LW/UW word marking. 2x transmit fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>0: disable LW/UW word marking. 1x transmit fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>2’b0</t>
+  </si>
+  <si>
+    <t>tx_fifo_mode:</t>
+  </si>
+  <si>
+    <t>00: transmit 1x fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>01: transmit 2x fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>11: transmit register mode.</t>
+  </si>
+  <si>
+    <t>20’b0</t>
+  </si>
+  <si>
+    <t>txswap_en:(only used in fifo 2x mode. This bit can not be set to “1” in register mode and fifo 1x mode)</t>
+  </si>
+  <si>
+    <t>1:The upper/lower word(bit[77:39]/bit[38:0])  of the transmit data from MAC(data_in[77:0], refer to table  3) is swapped. The upper/lower word of the loopback data in loopback path 1(Figure 9) is also swapped in 2x fifo loopback path 1 mode.</t>
+  </si>
+  <si>
+    <t>0x21c</t>
+  </si>
+  <si>
+    <t>16’b0</t>
+  </si>
+  <si>
+    <t>r_tx_adapter_lpbk_mode:</t>
+  </si>
+  <si>
+    <t>loop back path 2 and 3 mode.</t>
+  </si>
+  <si>
+    <t>00: no Loop back on loop back path 2 and  3</t>
+  </si>
+  <si>
+    <t>01: loop back path  2 enable</t>
+  </si>
+  <si>
+    <t>10: loop back path 3 enable, register mode</t>
+  </si>
+  <si>
+    <t>11: loop back path 3 enable,  fifo mode</t>
+  </si>
+  <si>
+    <t>13’b0</t>
+  </si>
+  <si>
+    <t>tx_double_write:</t>
+  </si>
+  <si>
+    <t>1:Transmit fifo write 2x width. 2x transmit fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t>0: Transmit fifo write 1x width. 1x transmit fifo phase comp mode.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">26     </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3844,6 +3996,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -3908,7 +4066,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -4070,11 +4228,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4605,6 +4833,60 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="46" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5077,7 +5359,7 @@
         <xdr:cNvPr id="2" name="Arrow: Curved Right 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5145,7 +5427,7 @@
         <xdr:cNvPr id="3" name="Arrow: Curved Right 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5533,7 +5815,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -5548,7 +5830,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -5722,7 +6004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD4A5BF-E111-4256-BC0D-F7B465E4781E}">
   <dimension ref="A1:H836"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C149" sqref="C149"/>
     </sheetView>
   </sheetViews>
@@ -5752,7 +6034,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -5764,7 +6046,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -7025,7 +7307,7 @@
       <c r="C80" s="143"/>
       <c r="D80" s="29"/>
       <c r="E80" s="29" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F80" s="21" t="s">
         <v>171</v>
@@ -7057,7 +7339,7 @@
       <c r="C82" s="144"/>
       <c r="D82" s="35"/>
       <c r="E82" s="35" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="F82" s="21" t="s">
         <v>171</v>
@@ -7494,7 +7776,7 @@
         <v>224</v>
       </c>
       <c r="F114" s="21" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="G114" s="26"/>
       <c r="H114" s="21"/>
@@ -7524,7 +7806,7 @@
         <v>228</v>
       </c>
       <c r="F116" s="21" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="G116" s="26"/>
       <c r="H116" s="21"/>
@@ -7554,7 +7836,7 @@
         <v>232</v>
       </c>
       <c r="F118" s="21" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="G118" s="26"/>
       <c r="H118" s="21"/>
@@ -7740,7 +8022,7 @@
         <v>256</v>
       </c>
       <c r="F130" s="25" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="G130" s="26"/>
       <c r="H130" s="21"/>
@@ -7800,7 +8082,7 @@
         <v>265</v>
       </c>
       <c r="F134" s="25" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="G134" s="26"/>
       <c r="H134" s="21"/>
@@ -7830,7 +8112,7 @@
         <v>269</v>
       </c>
       <c r="F136" s="25" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G136" s="26"/>
       <c r="H136" s="21"/>
@@ -8107,10 +8389,10 @@
         <v>310</v>
       </c>
       <c r="E154" s="25" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="F154" s="25" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G154" s="26"/>
       <c r="H154" s="21"/>
@@ -8122,7 +8404,7 @@
       <c r="D155" s="29"/>
       <c r="E155" s="35"/>
       <c r="F155" s="35" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="G155" s="26"/>
       <c r="H155" s="21"/>
@@ -8168,7 +8450,7 @@
         <v>316</v>
       </c>
       <c r="F158" s="23" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="G158" s="26"/>
       <c r="H158" s="21"/>
@@ -8180,7 +8462,7 @@
       <c r="D159" s="23"/>
       <c r="E159" s="21"/>
       <c r="F159" s="23" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="G159" s="26"/>
       <c r="H159" s="21"/>
@@ -8195,7 +8477,7 @@
         <v>318</v>
       </c>
       <c r="E160" s="23" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="F160" s="23"/>
       <c r="G160" s="26"/>
@@ -15046,8 +15328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B637F5-B6FF-4A8F-A0FE-E61D65E48007}">
   <dimension ref="A1:IV1016"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G178" sqref="G178"/>
+    <sheetView topLeftCell="A293" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B294" sqref="B294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15828,7 +16110,7 @@
     <row r="2" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -16087,7 +16369,7 @@
     <row r="3" spans="1:256" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -16715,7 +16997,7 @@
         <v>380</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -16739,7 +17021,7 @@
         <v>383</v>
       </c>
       <c r="F23" s="97" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="G23" s="57"/>
       <c r="H23" s="59"/>
@@ -16758,7 +17040,7 @@
         <v>386</v>
       </c>
       <c r="F24" s="98" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="G24" s="57"/>
       <c r="H24" s="59"/>
@@ -16777,7 +17059,7 @@
         <v>388</v>
       </c>
       <c r="F25" s="98" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="G25" s="57"/>
       <c r="H25" s="59"/>
@@ -16878,7 +17160,7 @@
         <v>404</v>
       </c>
       <c r="E31" s="63" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F31" s="100"/>
       <c r="G31" s="63"/>
@@ -17031,7 +17313,7 @@
         <v>426</v>
       </c>
       <c r="E40" s="63" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F40" s="100"/>
       <c r="G40" s="63"/>
@@ -17184,7 +17466,7 @@
         <v>450</v>
       </c>
       <c r="E49" s="63" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F49" s="100"/>
       <c r="G49" s="63"/>
@@ -17341,7 +17623,7 @@
         <v>476</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="F58" s="101"/>
       <c r="G58" s="11"/>
@@ -17498,7 +17780,7 @@
         <v>497</v>
       </c>
       <c r="E67" s="63" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="F67" s="100"/>
       <c r="G67" s="63"/>
@@ -17651,7 +17933,7 @@
         <v>514</v>
       </c>
       <c r="E76" s="63" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F76" s="100"/>
       <c r="G76" s="63"/>
@@ -17804,7 +18086,7 @@
         <v>535</v>
       </c>
       <c r="E85" s="63" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="F85" s="100"/>
       <c r="G85" s="63"/>
@@ -17977,13 +18259,13 @@
         <v>557</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="D96" s="45" t="s">
         <v>558</v>
       </c>
       <c r="E96" s="11" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="F96" s="101"/>
       <c r="G96" s="11"/>
@@ -18140,7 +18422,7 @@
         <v>573</v>
       </c>
       <c r="E105" s="63" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F105" s="100"/>
       <c r="G105" s="63"/>
@@ -18253,7 +18535,7 @@
       <c r="A112" s="98"/>
       <c r="B112" s="98"/>
       <c r="C112" s="71" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D112" s="57" t="s">
         <v>586</v>
@@ -18293,7 +18575,7 @@
         <v>591</v>
       </c>
       <c r="E114" s="63" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="F114" s="100"/>
       <c r="G114" s="63"/>
@@ -18446,7 +18728,7 @@
         <v>615</v>
       </c>
       <c r="E123" s="63" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F123" s="100"/>
       <c r="G123" s="63"/>
@@ -18698,7 +18980,7 @@
         <v>649</v>
       </c>
       <c r="F138" s="80" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="G138" s="80"/>
       <c r="H138" s="81"/>
@@ -18717,7 +18999,7 @@
         <v>652</v>
       </c>
       <c r="F139" s="80" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="G139" s="80"/>
       <c r="H139" s="81"/>
@@ -18736,7 +19018,7 @@
         <v>655</v>
       </c>
       <c r="F140" s="80" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="G140" s="80"/>
       <c r="H140" s="81"/>
@@ -18852,7 +19134,7 @@
         <v>668</v>
       </c>
       <c r="F148" s="80" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G148" s="80"/>
       <c r="H148" s="81"/>
@@ -18871,7 +19153,7 @@
         <v>671</v>
       </c>
       <c r="F149" s="80" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G149" s="80"/>
       <c r="H149" s="81"/>
@@ -18890,7 +19172,7 @@
         <v>674</v>
       </c>
       <c r="F150" s="80" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="G150" s="80"/>
       <c r="H150" s="81"/>
@@ -19055,7 +19337,7 @@
         <v>690</v>
       </c>
       <c r="E160" s="34" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="F160" s="21"/>
       <c r="G160" s="21"/>
@@ -19089,7 +19371,7 @@
         <v>694</v>
       </c>
       <c r="E162" s="109" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F162" s="23" t="s">
         <v>695</v>
@@ -19275,16 +19557,16 @@
       <c r="A174" s="35"/>
       <c r="B174" s="35"/>
       <c r="C174" s="128" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="D174" s="114" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="E174" s="114" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F174" s="21" t="s">
         <v>1228</v>
-      </c>
-      <c r="F174" s="21" t="s">
-        <v>1229</v>
       </c>
       <c r="G174" s="21"/>
       <c r="H174" s="26"/>
@@ -19296,10 +19578,10 @@
       <c r="C175" s="129"/>
       <c r="D175" s="115"/>
       <c r="E175" s="115" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="F175" s="21" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="G175" s="21"/>
       <c r="H175" s="26"/>
@@ -19323,7 +19605,7 @@
         <v>414</v>
       </c>
       <c r="D177" s="30" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="E177" s="30"/>
       <c r="F177" s="21"/>
@@ -19338,7 +19620,7 @@
         <v>417</v>
       </c>
       <c r="D178" s="30" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="E178" s="30" t="s">
         <v>19</v>
@@ -19352,7 +19634,7 @@
       <c r="A179" s="132"/>
       <c r="B179" s="132"/>
       <c r="C179" s="91" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="D179" s="23" t="s">
         <v>712</v>
@@ -19384,7 +19666,7 @@
       <c r="A181" s="132"/>
       <c r="B181" s="132"/>
       <c r="C181" s="93" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="D181" s="34" t="s">
         <v>715</v>
@@ -19420,7 +19702,7 @@
         <v>718</v>
       </c>
       <c r="E183" s="114" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F183" s="21" t="s">
         <v>719</v>
@@ -19604,7 +19886,7 @@
         <v>745</v>
       </c>
       <c r="F194" s="23" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="G194" s="21"/>
       <c r="H194" s="26"/>
@@ -19617,7 +19899,7 @@
       <c r="D195" s="29"/>
       <c r="E195" s="29"/>
       <c r="F195" s="23" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="G195" s="21"/>
       <c r="H195" s="26"/>
@@ -20453,10 +20735,10 @@
         <v>824</v>
       </c>
       <c r="E246" s="24" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F246" s="21" t="s">
         <v>1006</v>
-      </c>
-      <c r="F246" s="21" t="s">
-        <v>1007</v>
       </c>
       <c r="G246" s="21"/>
       <c r="H246" s="26"/>
@@ -20469,7 +20751,7 @@
       <c r="D247" s="38"/>
       <c r="E247" s="38"/>
       <c r="F247" s="21" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="G247" s="21"/>
       <c r="H247" s="26"/>
@@ -20482,7 +20764,7 @@
         <v>825</v>
       </c>
       <c r="D248" s="24" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="E248" s="24" t="s">
         <v>725</v>
@@ -20501,7 +20783,7 @@
       <c r="D249" s="38"/>
       <c r="E249" s="38"/>
       <c r="F249" s="21" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="G249" s="21"/>
       <c r="H249" s="26"/>
@@ -21192,10 +21474,10 @@
       <c r="A293" s="35"/>
       <c r="B293" s="35"/>
       <c r="C293" s="96" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D293" s="46" t="s">
         <v>902</v>
-      </c>
-      <c r="D293" s="46" t="s">
-        <v>903</v>
       </c>
       <c r="E293" s="23" t="s">
         <v>19</v>
@@ -21209,16 +21491,16 @@
       <c r="A294" s="132"/>
       <c r="B294" s="132"/>
       <c r="C294" s="150" t="s">
-        <v>302</v>
+        <v>1283</v>
       </c>
       <c r="D294" s="151" t="s">
+        <v>903</v>
+      </c>
+      <c r="E294" s="151" t="s">
         <v>904</v>
       </c>
-      <c r="E294" s="151" t="s">
+      <c r="F294" s="152" t="s">
         <v>905</v>
-      </c>
-      <c r="F294" s="152" t="s">
-        <v>906</v>
       </c>
       <c r="G294" s="90"/>
       <c r="H294" s="92"/>
@@ -21231,13 +21513,13 @@
         <v>653</v>
       </c>
       <c r="D295" s="46" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E295" s="46" t="s">
         <v>1011</v>
       </c>
-      <c r="E295" s="46" t="s">
-        <v>1012</v>
-      </c>
       <c r="F295" s="23" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="G295" s="90"/>
       <c r="H295" s="92"/>
@@ -21250,7 +21532,7 @@
         <v>708</v>
       </c>
       <c r="D296" s="16" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E296" s="16"/>
       <c r="F296" s="16"/>
@@ -21267,13 +21549,13 @@
         <v>708</v>
       </c>
       <c r="D297" s="23" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E297" s="23" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F297" s="23" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="G297" s="90"/>
       <c r="H297" s="92"/>
@@ -21286,7 +21568,7 @@
         <v>846</v>
       </c>
       <c r="D298" s="86" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E298" s="86"/>
       <c r="F298" s="16"/>
@@ -21303,13 +21585,13 @@
         <v>846</v>
       </c>
       <c r="D299" s="34" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E299" s="34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F299" s="23" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="G299" s="90"/>
       <c r="H299" s="92"/>
@@ -21322,7 +21604,7 @@
         <v>534</v>
       </c>
       <c r="D300" s="86" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E300" s="86"/>
       <c r="F300" s="16"/>
@@ -21336,16 +21618,16 @@
       <c r="A301" s="132"/>
       <c r="B301" s="132"/>
       <c r="C301" s="48" t="s">
+        <v>911</v>
+      </c>
+      <c r="D301" s="34" t="s">
         <v>912</v>
       </c>
-      <c r="D301" s="34" t="s">
-        <v>913</v>
-      </c>
       <c r="E301" s="34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F301" s="23" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="G301" s="90"/>
       <c r="H301" s="92"/>
@@ -21355,16 +21637,16 @@
       <c r="A302" s="35"/>
       <c r="B302" s="35"/>
       <c r="C302" s="125" t="s">
+        <v>913</v>
+      </c>
+      <c r="D302" s="109" t="s">
         <v>914</v>
       </c>
-      <c r="D302" s="109" t="s">
+      <c r="E302" s="109" t="s">
         <v>915</v>
       </c>
-      <c r="E302" s="109" t="s">
+      <c r="F302" s="23" t="s">
         <v>916</v>
-      </c>
-      <c r="F302" s="23" t="s">
-        <v>917</v>
       </c>
       <c r="G302" s="21" t="s">
         <v>639</v>
@@ -21379,7 +21661,7 @@
       <c r="D303" s="108"/>
       <c r="E303" s="108"/>
       <c r="F303" s="21" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G303" s="21"/>
       <c r="H303" s="26"/>
@@ -21389,7 +21671,7 @@
       <c r="A304" s="35"/>
       <c r="B304" s="35"/>
       <c r="C304" s="41" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D304" s="33" t="s">
         <v>19</v>
@@ -21409,7 +21691,7 @@
         <v>746</v>
       </c>
       <c r="D305" s="33" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E305" s="34" t="s">
         <v>19</v>
@@ -21421,21 +21703,21 @@
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="B306" s="11" t="s">
         <v>921</v>
-      </c>
-      <c r="B306" s="11" t="s">
-        <v>922</v>
       </c>
       <c r="C306" s="12" t="s">
         <v>475</v>
       </c>
       <c r="D306" s="45" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E306" s="45"/>
       <c r="F306" s="11"/>
       <c r="G306" s="11" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="H306" s="13" t="s">
         <v>31</v>
@@ -21448,7 +21730,7 @@
       <c r="A307" s="25"/>
       <c r="B307" s="25"/>
       <c r="C307" s="88" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D307" s="30" t="s">
         <v>19</v>
@@ -21465,13 +21747,13 @@
       <c r="A308" s="35"/>
       <c r="B308" s="35"/>
       <c r="C308" s="118" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D308" s="116" t="s">
         <v>676</v>
       </c>
       <c r="E308" s="116" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F308" s="23" t="s">
         <v>678</v>
@@ -21503,7 +21785,7 @@
         <v>680</v>
       </c>
       <c r="E310" s="116" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F310" s="23" t="s">
         <v>678</v>
@@ -21535,7 +21817,7 @@
         <v>683</v>
       </c>
       <c r="E312" s="116" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F312" s="23" t="s">
         <v>678</v>
@@ -21561,13 +21843,13 @@
       <c r="A314" s="35"/>
       <c r="B314" s="35"/>
       <c r="C314" s="118" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="D314" s="116" t="s">
         <v>767</v>
       </c>
       <c r="E314" s="116" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F314" s="23" t="s">
         <v>764</v>
@@ -21593,13 +21875,13 @@
       <c r="A316" s="35"/>
       <c r="B316" s="35"/>
       <c r="C316" s="118" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D316" s="116" t="s">
         <v>770</v>
       </c>
       <c r="E316" s="116" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F316" s="21" t="s">
         <v>764</v>
@@ -21631,7 +21913,7 @@
         <v>771</v>
       </c>
       <c r="E318" s="116" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F318" s="23" t="s">
         <v>764</v>
@@ -21663,7 +21945,7 @@
         <v>690</v>
       </c>
       <c r="E320" s="122" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F320" s="21"/>
       <c r="G320" s="21"/>
@@ -21677,12 +21959,12 @@
         <v>127</v>
       </c>
       <c r="D321" s="16" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E321" s="16"/>
       <c r="F321" s="16"/>
       <c r="G321" s="16" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="H321" s="19"/>
       <c r="I321" s="16"/>
@@ -21691,16 +21973,16 @@
       <c r="A322" s="35"/>
       <c r="B322" s="35"/>
       <c r="C322" s="120" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D322" s="97" t="s">
         <v>694</v>
       </c>
       <c r="E322" s="123" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F322" s="60" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="G322" s="21"/>
       <c r="H322" s="26"/>
@@ -21713,7 +21995,7 @@
       <c r="D323" s="102"/>
       <c r="E323" s="124"/>
       <c r="F323" s="60" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G323" s="21"/>
       <c r="H323" s="26"/>
@@ -21723,16 +22005,16 @@
       <c r="A324" s="35"/>
       <c r="B324" s="35"/>
       <c r="C324" s="120" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D324" s="25" t="s">
         <v>697</v>
       </c>
       <c r="E324" s="24" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F324" s="23" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="G324" s="21"/>
       <c r="H324" s="26"/>
@@ -21745,7 +22027,7 @@
       <c r="D325" s="29"/>
       <c r="E325" s="29"/>
       <c r="F325" s="23" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G325" s="21"/>
       <c r="H325" s="26"/>
@@ -21755,16 +22037,16 @@
       <c r="A326" s="35"/>
       <c r="B326" s="35"/>
       <c r="C326" s="125" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D326" s="25" t="s">
         <v>701</v>
       </c>
       <c r="E326" s="25" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F326" s="23" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="G326" s="21"/>
       <c r="H326" s="26"/>
@@ -21777,7 +22059,7 @@
       <c r="D327" s="29"/>
       <c r="E327" s="38"/>
       <c r="F327" s="21" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G327" s="21"/>
       <c r="H327" s="26"/>
@@ -21790,7 +22072,7 @@
         <v>590</v>
       </c>
       <c r="D328" s="86" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E328" s="86"/>
       <c r="F328" s="16"/>
@@ -21804,7 +22086,7 @@
       <c r="A329" s="35"/>
       <c r="B329" s="35"/>
       <c r="C329" s="41" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D329" s="33" t="s">
         <v>19</v>
@@ -21821,10 +22103,10 @@
       <c r="A330" s="35"/>
       <c r="B330" s="35"/>
       <c r="C330" s="41" t="s">
+        <v>939</v>
+      </c>
+      <c r="D330" s="34" t="s">
         <v>940</v>
-      </c>
-      <c r="D330" s="34" t="s">
-        <v>941</v>
       </c>
       <c r="E330" s="34" t="s">
         <v>19</v>
@@ -21841,7 +22123,7 @@
         <v>534</v>
       </c>
       <c r="D331" s="86" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E331" s="86"/>
       <c r="F331" s="16"/>
@@ -21855,7 +22137,7 @@
       <c r="A332" s="35"/>
       <c r="B332" s="35"/>
       <c r="C332" s="41" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D332" s="33" t="s">
         <v>19</v>
@@ -21872,10 +22154,10 @@
       <c r="A333" s="29"/>
       <c r="B333" s="29"/>
       <c r="C333" s="41" t="s">
+        <v>943</v>
+      </c>
+      <c r="D333" s="33" t="s">
         <v>944</v>
-      </c>
-      <c r="D333" s="33" t="s">
-        <v>945</v>
       </c>
       <c r="E333" s="34" t="s">
         <v>19</v>
@@ -21887,16 +22169,16 @@
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" s="11" t="s">
+        <v>945</v>
+      </c>
+      <c r="B334" s="11" t="s">
         <v>946</v>
-      </c>
-      <c r="B334" s="11" t="s">
-        <v>947</v>
       </c>
       <c r="C334" s="12" t="s">
         <v>379</v>
       </c>
       <c r="D334" s="45" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E334" s="45"/>
       <c r="F334" s="11"/>
@@ -21932,7 +22214,7 @@
         <v>708</v>
       </c>
       <c r="D336" s="16" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E336" s="16"/>
       <c r="F336" s="16"/>
@@ -21964,12 +22246,12 @@
         <v>846</v>
       </c>
       <c r="D338" s="86" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="E338" s="86"/>
       <c r="F338" s="16"/>
       <c r="G338" s="16" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H338" s="19"/>
       <c r="I338" s="16"/>
@@ -21978,7 +22260,7 @@
       <c r="A339" s="35"/>
       <c r="B339" s="35"/>
       <c r="C339" s="41" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D339" s="33" t="s">
         <v>19</v>
@@ -21998,10 +22280,10 @@
         <v>435</v>
       </c>
       <c r="D340" s="109" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="E340" s="106" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F340" s="23" t="s">
         <v>678</v>
@@ -22030,10 +22312,10 @@
         <v>863</v>
       </c>
       <c r="D342" s="109" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E342" s="106" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F342" s="23" t="s">
         <v>764</v>
@@ -22049,7 +22331,7 @@
       <c r="D343" s="108"/>
       <c r="E343" s="108"/>
       <c r="F343" s="23" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G343" s="21"/>
       <c r="H343" s="26"/>
@@ -22059,16 +22341,16 @@
       <c r="A344" s="35"/>
       <c r="B344" s="35"/>
       <c r="C344" s="125" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="D344" s="109" t="s">
         <v>701</v>
       </c>
       <c r="E344" s="106" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F344" s="23" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="G344" s="21"/>
       <c r="H344" s="26"/>
@@ -22081,7 +22363,7 @@
       <c r="D345" s="108"/>
       <c r="E345" s="108"/>
       <c r="F345" s="23" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="G345" s="21"/>
       <c r="H345" s="26"/>
@@ -22094,7 +22376,7 @@
         <v>691</v>
       </c>
       <c r="D346" s="86" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E346" s="86"/>
       <c r="F346" s="16"/>
@@ -22121,13 +22403,13 @@
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A348" s="11" t="s">
+        <v>957</v>
+      </c>
+      <c r="B348" s="11" t="s">
         <v>958</v>
       </c>
-      <c r="B348" s="11" t="s">
+      <c r="C348" s="12" t="s">
         <v>959</v>
-      </c>
-      <c r="C348" s="12" t="s">
-        <v>960</v>
       </c>
       <c r="D348" s="45" t="s">
         <v>19</v>
@@ -22144,13 +22426,13 @@
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A349" s="11" t="s">
+        <v>960</v>
+      </c>
+      <c r="B349" s="11" t="s">
         <v>961</v>
       </c>
-      <c r="B349" s="11" t="s">
-        <v>962</v>
-      </c>
       <c r="C349" s="50" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D349" s="11" t="s">
         <v>19</v>
@@ -22167,13 +22449,13 @@
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A350" s="11" t="s">
+        <v>962</v>
+      </c>
+      <c r="B350" s="11" t="s">
         <v>963</v>
       </c>
-      <c r="B350" s="11" t="s">
-        <v>964</v>
-      </c>
       <c r="C350" s="50" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D350" s="11" t="s">
         <v>19</v>
@@ -22190,10 +22472,10 @@
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A351" s="11" t="s">
+        <v>964</v>
+      </c>
+      <c r="B351" s="11" t="s">
         <v>965</v>
-      </c>
-      <c r="B351" s="11" t="s">
-        <v>966</v>
       </c>
       <c r="C351" s="50" t="s">
         <v>342</v>
@@ -29572,16 +29854,16 @@
       <c r="I1" s="153"/>
     </row>
     <row r="2" spans="2:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="184" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
+      <c r="B2" s="202" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
       <c r="G2" s="154"/>
       <c r="H2" s="155" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="I2" s="155"/>
     </row>
@@ -29593,19 +29875,19 @@
     </row>
     <row r="4" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="156" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C4" s="157" t="s">
         <v>1015</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="D4" s="157" t="s">
         <v>1016</v>
       </c>
-      <c r="D4" s="157" t="s">
+      <c r="E4" s="158" t="s">
         <v>1017</v>
       </c>
-      <c r="E4" s="158" t="s">
+      <c r="F4" s="159" t="s">
         <v>1018</v>
-      </c>
-      <c r="F4" s="159" t="s">
-        <v>1019</v>
       </c>
       <c r="G4" s="154"/>
       <c r="H4" s="154"/>
@@ -29616,16 +29898,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="161" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D5" s="162" t="s">
         <v>1020</v>
       </c>
-      <c r="D5" s="162" t="s">
+      <c r="E5" s="163" t="s">
         <v>1021</v>
       </c>
-      <c r="E5" s="163" t="s">
+      <c r="F5" s="164" t="s">
         <v>1022</v>
-      </c>
-      <c r="F5" s="164" t="s">
-        <v>1023</v>
       </c>
       <c r="G5" s="165"/>
       <c r="H5" s="165"/>
@@ -29636,16 +29918,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="167" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D6" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E6" s="163" t="s">
         <v>1024</v>
       </c>
-      <c r="D6" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E6" s="163" t="s">
+      <c r="F6" s="164" t="s">
         <v>1025</v>
-      </c>
-      <c r="F6" s="164" t="s">
-        <v>1026</v>
       </c>
       <c r="G6" s="165"/>
       <c r="H6" s="165"/>
@@ -29656,16 +29938,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="167" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D7" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E7" s="163" t="s">
         <v>1027</v>
       </c>
-      <c r="D7" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E7" s="163" t="s">
-        <v>1028</v>
-      </c>
       <c r="F7" s="164" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G7" s="169"/>
       <c r="H7" s="169"/>
@@ -29674,16 +29956,16 @@
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="166"/>
       <c r="C8" s="167" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D8" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E8" s="163" t="s">
         <v>1029</v>
       </c>
-      <c r="D8" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E8" s="163" t="s">
-        <v>1030</v>
-      </c>
       <c r="F8" s="164" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G8" s="169"/>
       <c r="H8" s="169"/>
@@ -29692,16 +29974,16 @@
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="166"/>
       <c r="C9" s="167" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D9" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E9" s="163" t="s">
         <v>1031</v>
       </c>
-      <c r="D9" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E9" s="163" t="s">
-        <v>1032</v>
-      </c>
       <c r="F9" s="164" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G9" s="169"/>
       <c r="H9" s="169"/>
@@ -29710,16 +29992,16 @@
     <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="166"/>
       <c r="C10" s="167" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D10" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E10" s="163" t="s">
         <v>1033</v>
       </c>
-      <c r="D10" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E10" s="163" t="s">
-        <v>1034</v>
-      </c>
       <c r="F10" s="164" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G10" s="169"/>
       <c r="H10" s="169"/>
@@ -29728,16 +30010,16 @@
     <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="166"/>
       <c r="C11" s="167" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D11" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E11" s="163" t="s">
         <v>1035</v>
       </c>
-      <c r="D11" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E11" s="163" t="s">
-        <v>1036</v>
-      </c>
       <c r="F11" s="164" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G11" s="169"/>
       <c r="H11" s="169"/>
@@ -29746,16 +30028,16 @@
     <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="166"/>
       <c r="C12" s="167" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D12" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E12" s="163" t="s">
         <v>1037</v>
       </c>
-      <c r="D12" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E12" s="163" t="s">
-        <v>1038</v>
-      </c>
       <c r="F12" s="164" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G12" s="169"/>
       <c r="H12" s="169"/>
@@ -29764,16 +30046,16 @@
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="166"/>
       <c r="C13" s="167" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D13" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E13" s="163" t="s">
         <v>1039</v>
       </c>
-      <c r="D13" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E13" s="163" t="s">
-        <v>1040</v>
-      </c>
       <c r="F13" s="164" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G13" s="169"/>
       <c r="H13" s="169"/>
@@ -29782,16 +30064,16 @@
     <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="166"/>
       <c r="C14" s="167" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D14" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E14" s="170" t="s">
         <v>1041</v>
       </c>
-      <c r="D14" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E14" s="170" t="s">
+      <c r="F14" s="170" t="s">
         <v>1042</v>
-      </c>
-      <c r="F14" s="170" t="s">
-        <v>1043</v>
       </c>
       <c r="G14" s="169"/>
       <c r="H14" s="169"/>
@@ -29800,16 +30082,16 @@
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="166"/>
       <c r="C15" s="167" t="s">
+        <v>1043</v>
+      </c>
+      <c r="D15" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E15" s="163" t="s">
         <v>1044</v>
       </c>
-      <c r="D15" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E15" s="163" t="s">
-        <v>1045</v>
-      </c>
       <c r="F15" s="163" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G15" s="169"/>
       <c r="H15" s="169"/>
@@ -29818,13 +30100,13 @@
     <row r="16" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="166"/>
       <c r="C16" s="167" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D16" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E16" s="163" t="s">
         <v>1046</v>
-      </c>
-      <c r="D16" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E16" s="163" t="s">
-        <v>1047</v>
       </c>
       <c r="F16" s="163"/>
       <c r="G16" s="169"/>
@@ -29834,13 +30116,13 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="166"/>
       <c r="C17" s="167" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D17" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E17" s="163" t="s">
         <v>1048</v>
-      </c>
-      <c r="D17" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E17" s="163" t="s">
-        <v>1049</v>
       </c>
       <c r="F17" s="163"/>
       <c r="G17" s="169"/>
@@ -29850,13 +30132,13 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="166"/>
       <c r="C18" s="167" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D18" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E18" s="163" t="s">
         <v>1050</v>
-      </c>
-      <c r="D18" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E18" s="163" t="s">
-        <v>1051</v>
       </c>
       <c r="F18" s="163"/>
       <c r="G18" s="169"/>
@@ -29866,16 +30148,16 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="166"/>
       <c r="C19" s="167" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D19" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E19" s="163" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="F19" s="163" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="G19" s="169"/>
       <c r="H19" s="169"/>
@@ -29886,13 +30168,13 @@
         <v>4</v>
       </c>
       <c r="C20" s="167" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D20" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E20" s="163" t="s">
         <v>1053</v>
-      </c>
-      <c r="D20" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E20" s="163" t="s">
-        <v>1054</v>
       </c>
       <c r="F20" s="163"/>
       <c r="G20" s="169"/>
@@ -29904,13 +30186,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="167" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D21" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E21" s="163" t="s">
         <v>1055</v>
-      </c>
-      <c r="D21" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E21" s="163" t="s">
-        <v>1056</v>
       </c>
       <c r="F21" s="163"/>
       <c r="G21" s="169"/>
@@ -29922,13 +30204,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="167" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D22" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E22" s="163" t="s">
         <v>1057</v>
-      </c>
-      <c r="D22" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E22" s="163" t="s">
-        <v>1058</v>
       </c>
       <c r="F22" s="163"/>
       <c r="G22" s="169"/>
@@ -29940,13 +30222,13 @@
         <v>7</v>
       </c>
       <c r="C23" s="167" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D23" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E23" s="163" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="F23" s="163"/>
       <c r="G23" s="169"/>
@@ -29958,13 +30240,13 @@
         <v>8</v>
       </c>
       <c r="C24" s="167" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D24" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E24" s="163" t="s">
         <v>1060</v>
-      </c>
-      <c r="D24" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E24" s="163" t="s">
-        <v>1061</v>
       </c>
       <c r="F24" s="163"/>
       <c r="G24" s="169"/>
@@ -29976,16 +30258,16 @@
         <v>9</v>
       </c>
       <c r="C25" s="167" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D25" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E25" s="163" t="s">
         <v>1062</v>
       </c>
-      <c r="D25" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E25" s="163" t="s">
+      <c r="F25" s="163" t="s">
         <v>1063</v>
-      </c>
-      <c r="F25" s="163" t="s">
-        <v>1064</v>
       </c>
       <c r="G25" s="169"/>
       <c r="H25" s="169"/>
@@ -29999,10 +30281,10 @@
         <v>877</v>
       </c>
       <c r="D26" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E26" s="170" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="F26" s="170"/>
       <c r="G26" s="171"/>
@@ -30017,13 +30299,13 @@
         <v>872</v>
       </c>
       <c r="D27" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E27" s="170" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F27" s="163" t="s">
         <v>1066</v>
-      </c>
-      <c r="F27" s="163" t="s">
-        <v>1067</v>
       </c>
       <c r="G27" s="169"/>
       <c r="H27" s="169"/>
@@ -30034,13 +30316,13 @@
         <v>12</v>
       </c>
       <c r="C28" s="167" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D28" s="168" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E28" s="172" t="s">
         <v>1068</v>
-      </c>
-      <c r="D28" s="168" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E28" s="172" t="s">
-        <v>1069</v>
       </c>
       <c r="F28" s="172"/>
       <c r="G28" s="165"/>
@@ -30052,13 +30334,13 @@
         <v>13</v>
       </c>
       <c r="C29" s="167" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D29" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E29" s="163" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F29" s="163"/>
       <c r="G29" s="169"/>
@@ -30070,13 +30352,13 @@
         <v>14</v>
       </c>
       <c r="C30" s="167" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D30" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E30" s="163" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F30" s="163"/>
       <c r="G30" s="169"/>
@@ -30088,13 +30370,13 @@
         <v>15</v>
       </c>
       <c r="C31" s="167" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D31" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E31" s="163" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F31" s="163"/>
       <c r="G31" s="169"/>
@@ -30106,13 +30388,13 @@
         <v>16</v>
       </c>
       <c r="C32" s="167" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D32" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E32" s="163" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F32" s="163"/>
       <c r="G32" s="169"/>
@@ -30124,13 +30406,13 @@
         <v>17</v>
       </c>
       <c r="C33" s="167" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D33" s="168" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="E33" s="163" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F33" s="163"/>
       <c r="G33" s="169"/>
@@ -30146,13 +30428,13 @@
         <v>19</v>
       </c>
       <c r="C35" s="167" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D35" s="176" t="s">
         <v>1075</v>
       </c>
-      <c r="D35" s="176" t="s">
+      <c r="E35" s="163" t="s">
         <v>1076</v>
-      </c>
-      <c r="E35" s="163" t="s">
-        <v>1077</v>
       </c>
       <c r="F35" s="149"/>
       <c r="G35" s="149"/>
@@ -30162,11 +30444,11 @@
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="175"/>
       <c r="C36" s="167" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D36" s="176"/>
       <c r="E36" s="163" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="F36" s="149"/>
       <c r="G36" s="149"/>
@@ -30176,11 +30458,11 @@
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="167"/>
       <c r="C37" s="167" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D37" s="176"/>
       <c r="E37" s="163" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="F37" s="149"/>
       <c r="G37" s="149"/>
@@ -30190,11 +30472,11 @@
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="167"/>
       <c r="C38" s="167" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D38" s="176"/>
       <c r="E38" s="163" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F38" s="149"/>
       <c r="G38" s="149"/>
@@ -30206,16 +30488,16 @@
         <v>20</v>
       </c>
       <c r="C39" s="167" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D39" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E39" s="163" t="s">
         <v>1084</v>
       </c>
-      <c r="D39" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E39" s="163" t="s">
+      <c r="F39" s="149" t="s">
         <v>1085</v>
-      </c>
-      <c r="F39" s="149" t="s">
-        <v>1086</v>
       </c>
       <c r="G39" s="149"/>
       <c r="H39" s="149"/>
@@ -30226,16 +30508,16 @@
         <v>21</v>
       </c>
       <c r="C40" s="167" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D40" s="176" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E40" s="163" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F40" s="149" t="s">
         <v>1085</v>
-      </c>
-      <c r="F40" s="149" t="s">
-        <v>1086</v>
       </c>
       <c r="G40" s="149"/>
       <c r="H40" s="149"/>
@@ -30246,13 +30528,13 @@
         <v>22</v>
       </c>
       <c r="C41" s="167" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D41" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E41" s="163" t="s">
         <v>1088</v>
-      </c>
-      <c r="D41" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E41" s="163" t="s">
-        <v>1089</v>
       </c>
       <c r="F41" s="149"/>
       <c r="G41" s="149"/>
@@ -30264,13 +30546,13 @@
         <v>23</v>
       </c>
       <c r="C42" s="167" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D42" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E42" s="163" t="s">
         <v>1090</v>
-      </c>
-      <c r="D42" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E42" s="163" t="s">
-        <v>1091</v>
       </c>
       <c r="F42" s="149"/>
       <c r="G42" s="149"/>
@@ -30282,13 +30564,13 @@
         <v>24</v>
       </c>
       <c r="C43" s="167" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D43" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E43" s="163" t="s">
         <v>1092</v>
-      </c>
-      <c r="D43" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E43" s="163" t="s">
-        <v>1093</v>
       </c>
       <c r="F43" s="149"/>
       <c r="G43" s="149"/>
@@ -30300,13 +30582,13 @@
         <v>25</v>
       </c>
       <c r="C44" s="167" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D44" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E44" s="163" t="s">
         <v>1094</v>
-      </c>
-      <c r="D44" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E44" s="163" t="s">
-        <v>1095</v>
       </c>
       <c r="F44" s="149"/>
       <c r="G44" s="149"/>
@@ -30318,13 +30600,13 @@
         <v>26</v>
       </c>
       <c r="C45" s="167" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D45" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E45" s="163" t="s">
         <v>1096</v>
-      </c>
-      <c r="D45" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E45" s="163" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
@@ -30332,13 +30614,13 @@
         <v>27</v>
       </c>
       <c r="C46" s="167" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D46" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E46" s="163" t="s">
         <v>1098</v>
-      </c>
-      <c r="D46" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E46" s="163" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="47" spans="2:9" ht="30" x14ac:dyDescent="0.25">
@@ -30346,13 +30628,13 @@
         <v>28</v>
       </c>
       <c r="C47" s="167" t="s">
+        <v>1099</v>
+      </c>
+      <c r="D47" s="176" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E47" s="163" t="s">
         <v>1100</v>
-      </c>
-      <c r="D47" s="176" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E47" s="163" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
@@ -30360,10 +30642,10 @@
         <v>29</v>
       </c>
       <c r="C48" s="177" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D48" s="176" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E48" s="167"/>
     </row>
@@ -30378,363 +30660,363 @@
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="178" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D52" s="178" t="s">
         <v>1103</v>
       </c>
-      <c r="D52" s="178" t="s">
+      <c r="E52" s="178" t="s">
         <v>1104</v>
-      </c>
-      <c r="E52" s="178" t="s">
-        <v>1105</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" s="166" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D53" s="166" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E53" s="179"/>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" s="166" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D54" s="166" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E54" s="179"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C55" s="166" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D55" s="166" t="s">
         <v>1108</v>
       </c>
-      <c r="D55" s="166" t="s">
+      <c r="E55" s="180" t="s">
         <v>1109</v>
-      </c>
-      <c r="E55" s="180" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" s="166" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D56" s="166" t="s">
         <v>1111</v>
       </c>
-      <c r="D56" s="166" t="s">
+      <c r="E56" s="181" t="s">
         <v>1112</v>
-      </c>
-      <c r="E56" s="181" t="s">
-        <v>1113</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57" s="166"/>
       <c r="D57" s="166" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E57" s="180" t="s">
         <v>1114</v>
-      </c>
-      <c r="E57" s="180" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58" s="166"/>
       <c r="D58" s="166" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E58" s="180" t="s">
         <v>1116</v>
-      </c>
-      <c r="E58" s="180" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="166" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D59" s="166" t="s">
         <v>1118</v>
-      </c>
-      <c r="D59" s="166" t="s">
-        <v>1119</v>
       </c>
       <c r="E59" s="179"/>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="167"/>
       <c r="D60" s="175" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E60" s="182" t="s">
         <v>1120</v>
-      </c>
-      <c r="E60" s="182" t="s">
-        <v>1121</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" s="183" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D64" s="183" t="s">
         <v>1122</v>
       </c>
-      <c r="D64" s="183" t="s">
+      <c r="E64" s="183" t="s">
         <v>1123</v>
-      </c>
-      <c r="E64" s="183" t="s">
-        <v>1124</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65" s="166" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D65" s="166" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E65" s="166" t="s">
         <v>1125</v>
-      </c>
-      <c r="E65" s="166" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66" s="166"/>
       <c r="D66" s="166" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E66" s="166" t="s">
         <v>1127</v>
-      </c>
-      <c r="E66" s="166" t="s">
-        <v>1128</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C67" s="166"/>
       <c r="D67" s="166" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E67" s="166" t="s">
         <v>1129</v>
-      </c>
-      <c r="E67" s="166" t="s">
-        <v>1130</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C68" s="166"/>
       <c r="D68" s="166" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E68" s="166" t="s">
         <v>1131</v>
-      </c>
-      <c r="E68" s="166" t="s">
-        <v>1132</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C69" s="166" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D69" s="166" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E69" s="166" t="s">
         <v>1133</v>
-      </c>
-      <c r="E69" s="166" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C70" s="166"/>
       <c r="D70" s="166" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E70" s="166" t="s">
         <v>1135</v>
-      </c>
-      <c r="E70" s="166" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C71" s="166"/>
       <c r="D71" s="166" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E71" s="166" t="s">
         <v>1137</v>
-      </c>
-      <c r="E71" s="166" t="s">
-        <v>1138</v>
       </c>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C72" s="166"/>
       <c r="D72" s="166" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E72" s="166" t="s">
         <v>1139</v>
-      </c>
-      <c r="E72" s="166" t="s">
-        <v>1140</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73" s="166" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D73" s="166" t="s">
         <v>1141</v>
       </c>
-      <c r="D73" s="166" t="s">
+      <c r="E73" s="166" t="s">
         <v>1142</v>
-      </c>
-      <c r="E73" s="166" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C74" s="166"/>
       <c r="D74" s="166" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E74" s="166" t="s">
         <v>1144</v>
-      </c>
-      <c r="E74" s="166" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="75" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C75" s="166"/>
       <c r="D75" s="166" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E75" s="166" t="s">
         <v>1146</v>
-      </c>
-      <c r="E75" s="166" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="76" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C76" s="166"/>
       <c r="D76" s="166" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E76" s="166" t="s">
         <v>1148</v>
-      </c>
-      <c r="E76" s="166" t="s">
-        <v>1149</v>
       </c>
     </row>
     <row r="77" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C77" s="166" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D77" s="166" t="s">
         <v>1150</v>
       </c>
-      <c r="D77" s="166" t="s">
+      <c r="E77" s="166" t="s">
         <v>1151</v>
-      </c>
-      <c r="E77" s="166" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="78" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C78" s="166"/>
       <c r="D78" s="166" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E78" s="166" t="s">
         <v>1153</v>
-      </c>
-      <c r="E78" s="166" t="s">
-        <v>1154</v>
       </c>
     </row>
     <row r="79" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C79" s="166"/>
       <c r="D79" s="166" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E79" s="166" t="s">
         <v>1155</v>
-      </c>
-      <c r="E79" s="166" t="s">
-        <v>1156</v>
       </c>
     </row>
     <row r="80" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C80" s="166"/>
       <c r="D80" s="166" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E80" s="166" t="s">
         <v>1157</v>
-      </c>
-      <c r="E80" s="166" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81" s="166" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D81" s="166" t="s">
         <v>1159</v>
       </c>
-      <c r="D81" s="166" t="s">
+      <c r="E81" s="166" t="s">
         <v>1160</v>
-      </c>
-      <c r="E81" s="166" t="s">
-        <v>1161</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C82" s="166"/>
       <c r="D82" s="166" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E82" s="166" t="s">
         <v>1162</v>
-      </c>
-      <c r="E82" s="166" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C83" s="166"/>
       <c r="D83" s="166" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E83" s="166" t="s">
         <v>1164</v>
-      </c>
-      <c r="E83" s="166" t="s">
-        <v>1165</v>
       </c>
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C84" s="166"/>
       <c r="D84" s="166" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E84" s="166" t="s">
         <v>1166</v>
-      </c>
-      <c r="E84" s="166" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C85" s="166" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D85" s="166" t="s">
         <v>1168</v>
       </c>
-      <c r="D85" s="166" t="s">
+      <c r="E85" s="166" t="s">
         <v>1169</v>
-      </c>
-      <c r="E85" s="166" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C86" s="166"/>
       <c r="D86" s="166" t="s">
+        <v>1170</v>
+      </c>
+      <c r="E86" s="166" t="s">
         <v>1171</v>
-      </c>
-      <c r="E86" s="166" t="s">
-        <v>1172</v>
       </c>
     </row>
     <row r="87" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C87" s="166"/>
       <c r="D87" s="166" t="s">
+        <v>1172</v>
+      </c>
+      <c r="E87" s="166" t="s">
         <v>1173</v>
-      </c>
-      <c r="E87" s="166" t="s">
-        <v>1174</v>
       </c>
     </row>
     <row r="88" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C88" s="166"/>
       <c r="D88" s="166" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E88" s="166" t="s">
         <v>1175</v>
-      </c>
-      <c r="E88" s="166" t="s">
-        <v>1176</v>
       </c>
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C89" s="166" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D89" s="166" t="s">
         <v>1177</v>
       </c>
-      <c r="D89" s="166" t="s">
+      <c r="E89" s="166" t="s">
         <v>1178</v>
-      </c>
-      <c r="E89" s="166" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="90" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C90" s="166"/>
       <c r="D90" s="166" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E90" s="166" t="s">
         <v>1180</v>
-      </c>
-      <c r="E90" s="166" t="s">
-        <v>1181</v>
       </c>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C91" s="166"/>
       <c r="D91" s="166" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E91" s="166" t="s">
         <v>1182</v>
-      </c>
-      <c r="E91" s="166" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="92" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C92" s="166"/>
       <c r="D92" s="166" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="E92" s="166">
         <v>0</v>
@@ -30742,37 +31024,37 @@
     </row>
     <row r="93" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C93" s="166" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D93" s="166" t="s">
         <v>1185</v>
       </c>
-      <c r="D93" s="166" t="s">
+      <c r="E93" s="166" t="s">
         <v>1186</v>
-      </c>
-      <c r="E93" s="166" t="s">
-        <v>1187</v>
       </c>
     </row>
     <row r="94" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C94" s="166"/>
       <c r="D94" s="166" t="s">
+        <v>1187</v>
+      </c>
+      <c r="E94" s="166" t="s">
         <v>1188</v>
-      </c>
-      <c r="E94" s="166" t="s">
-        <v>1189</v>
       </c>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C95" s="166"/>
       <c r="D95" s="166" t="s">
+        <v>1189</v>
+      </c>
+      <c r="E95" s="166" t="s">
         <v>1190</v>
-      </c>
-      <c r="E95" s="166" t="s">
-        <v>1191</v>
       </c>
     </row>
     <row r="96" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C96" s="166"/>
       <c r="D96" s="166" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="E96" s="166">
         <v>0</v>
@@ -30780,37 +31062,37 @@
     </row>
     <row r="97" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C97" s="166" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D97" s="166" t="s">
         <v>1193</v>
       </c>
-      <c r="D97" s="166" t="s">
+      <c r="E97" s="166" t="s">
         <v>1194</v>
-      </c>
-      <c r="E97" s="166" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="98" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C98" s="166"/>
       <c r="D98" s="166" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E98" s="166" t="s">
         <v>1196</v>
-      </c>
-      <c r="E98" s="166" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="99" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C99" s="166"/>
       <c r="D99" s="166" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E99" s="166" t="s">
         <v>1198</v>
-      </c>
-      <c r="E99" s="166" t="s">
-        <v>1199</v>
       </c>
     </row>
     <row r="100" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C100" s="166"/>
       <c r="D100" s="166" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="E100" s="166">
         <v>0</v>
@@ -30818,37 +31100,37 @@
     </row>
     <row r="101" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C101" s="166" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D101" s="166" t="s">
         <v>1201</v>
       </c>
-      <c r="D101" s="166" t="s">
+      <c r="E101" s="166" t="s">
         <v>1202</v>
-      </c>
-      <c r="E101" s="166" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="102" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C102" s="166"/>
       <c r="D102" s="166" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E102" s="166" t="s">
         <v>1204</v>
-      </c>
-      <c r="E102" s="166" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="103" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C103" s="166"/>
       <c r="D103" s="166" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E103" s="166" t="s">
         <v>1206</v>
-      </c>
-      <c r="E103" s="166" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="104" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C104" s="166"/>
       <c r="D104" s="166" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="E104" s="166">
         <v>0</v>
@@ -30856,37 +31138,37 @@
     </row>
     <row r="105" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C105" s="166" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D105" s="166" t="s">
         <v>1209</v>
       </c>
-      <c r="D105" s="166" t="s">
+      <c r="E105" s="166" t="s">
         <v>1210</v>
-      </c>
-      <c r="E105" s="166" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="106" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C106" s="166"/>
       <c r="D106" s="166" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E106" s="166" t="s">
         <v>1212</v>
-      </c>
-      <c r="E106" s="166" t="s">
-        <v>1213</v>
       </c>
     </row>
     <row r="107" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C107" s="166"/>
       <c r="D107" s="166" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E107" s="166" t="s">
         <v>1214</v>
-      </c>
-      <c r="E107" s="166" t="s">
-        <v>1215</v>
       </c>
     </row>
     <row r="108" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C108" s="166"/>
       <c r="D108" s="166" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="E108" s="166">
         <v>0</v>
@@ -30898,6 +31180,651 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F2E58B-D011-4FB9-988B-7747060B50FE}">
+  <dimension ref="A1:F45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="196" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="196" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="184">
+        <v>1.3111111111111111</v>
+      </c>
+      <c r="D1" s="185" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="185" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F1" s="185" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="197"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="196">
+        <v>27</v>
+      </c>
+      <c r="D2" s="196" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="196" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F2" s="191" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="197"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="191" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="197"/>
+      <c r="B4" s="197"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="192" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="197"/>
+      <c r="B5" s="197"/>
+      <c r="C5" s="188">
+        <v>1.0840277777777778</v>
+      </c>
+      <c r="D5" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="187" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F5" s="187" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="197"/>
+      <c r="B6" s="197"/>
+      <c r="C6" s="196">
+        <v>0</v>
+      </c>
+      <c r="D6" s="196" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="196" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F6" s="191" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="197"/>
+      <c r="B7" s="197"/>
+      <c r="C7" s="197"/>
+      <c r="D7" s="197"/>
+      <c r="E7" s="197"/>
+      <c r="F7" s="191" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="198"/>
+      <c r="B8" s="198"/>
+      <c r="C8" s="198"/>
+      <c r="D8" s="198"/>
+      <c r="E8" s="198"/>
+      <c r="F8" s="192" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="196" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="196" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C9" s="188">
+        <v>1.2965277777777777</v>
+      </c>
+      <c r="D9" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="187" t="s">
+        <v>1244</v>
+      </c>
+      <c r="F9" s="187" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="197"/>
+      <c r="B10" s="197"/>
+      <c r="C10" s="193">
+        <v>6</v>
+      </c>
+      <c r="D10" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="193" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F10" s="186" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="197"/>
+      <c r="B11" s="197"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="194"/>
+      <c r="E11" s="194"/>
+      <c r="F11" s="186" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="197"/>
+      <c r="B12" s="197"/>
+      <c r="C12" s="194"/>
+      <c r="D12" s="194"/>
+      <c r="E12" s="194"/>
+      <c r="F12" s="186" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="197"/>
+      <c r="B13" s="197"/>
+      <c r="C13" s="195"/>
+      <c r="D13" s="195"/>
+      <c r="E13" s="195"/>
+      <c r="F13" s="187"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="198"/>
+      <c r="B14" s="198"/>
+      <c r="C14" s="189">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D14" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="187" t="s">
+        <v>1248</v>
+      </c>
+      <c r="F14" s="187" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="196" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="196" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="188">
+        <v>1.29375</v>
+      </c>
+      <c r="D15" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="187" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F15" s="187" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="197"/>
+      <c r="B16" s="197"/>
+      <c r="C16" s="199">
+        <v>8.4027777777777771E-2</v>
+      </c>
+      <c r="D16" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="193" t="s">
+        <v>1250</v>
+      </c>
+      <c r="F16" s="186" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="197"/>
+      <c r="B17" s="197"/>
+      <c r="C17" s="200"/>
+      <c r="D17" s="194"/>
+      <c r="E17" s="194"/>
+      <c r="F17" s="186" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="197"/>
+      <c r="B18" s="197"/>
+      <c r="C18" s="200"/>
+      <c r="D18" s="194"/>
+      <c r="E18" s="194"/>
+      <c r="F18" s="186" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="197"/>
+      <c r="B19" s="197"/>
+      <c r="C19" s="201"/>
+      <c r="D19" s="195"/>
+      <c r="E19" s="195"/>
+      <c r="F19" s="187" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="197"/>
+      <c r="B20" s="197"/>
+      <c r="C20" s="193">
+        <v>0</v>
+      </c>
+      <c r="D20" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="193" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F20" s="186" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="197"/>
+      <c r="B21" s="197"/>
+      <c r="C21" s="194"/>
+      <c r="D21" s="194"/>
+      <c r="E21" s="194"/>
+      <c r="F21" s="186" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="198"/>
+      <c r="B22" s="198"/>
+      <c r="C22" s="195"/>
+      <c r="D22" s="195"/>
+      <c r="E22" s="195"/>
+      <c r="F22" s="187" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="196" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="196" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="188">
+        <v>1.3083333333333333</v>
+      </c>
+      <c r="D23" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="187" t="s">
+        <v>1258</v>
+      </c>
+      <c r="F23" s="187" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="197"/>
+      <c r="B24" s="197"/>
+      <c r="C24" s="193">
+        <v>23</v>
+      </c>
+      <c r="D24" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="193" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F24" s="186" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="197"/>
+      <c r="B25" s="197"/>
+      <c r="C25" s="194"/>
+      <c r="D25" s="194"/>
+      <c r="E25" s="194"/>
+      <c r="F25" s="186" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="197"/>
+      <c r="B26" s="197"/>
+      <c r="C26" s="195"/>
+      <c r="D26" s="195"/>
+      <c r="E26" s="195"/>
+      <c r="F26" s="187" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="197"/>
+      <c r="B27" s="197"/>
+      <c r="C27" s="199">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="D27" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="193" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F27" s="186" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="197"/>
+      <c r="B28" s="197"/>
+      <c r="C28" s="200"/>
+      <c r="D28" s="194"/>
+      <c r="E28" s="194"/>
+      <c r="F28" s="186" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="197"/>
+      <c r="B29" s="197"/>
+      <c r="C29" s="200"/>
+      <c r="D29" s="194"/>
+      <c r="E29" s="194"/>
+      <c r="F29" s="186" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="197"/>
+      <c r="B30" s="197"/>
+      <c r="C30" s="201"/>
+      <c r="D30" s="195"/>
+      <c r="E30" s="195"/>
+      <c r="F30" s="187" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="197"/>
+      <c r="B31" s="197"/>
+      <c r="C31" s="189">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="D31" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="187" t="s">
+        <v>1267</v>
+      </c>
+      <c r="F31" s="187" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="197"/>
+      <c r="B32" s="197"/>
+      <c r="C32" s="193">
+        <v>0</v>
+      </c>
+      <c r="D32" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="193" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F32" s="186" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="197"/>
+      <c r="B33" s="197"/>
+      <c r="C33" s="194"/>
+      <c r="D33" s="194"/>
+      <c r="E33" s="194"/>
+      <c r="F33" s="186" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="198"/>
+      <c r="B34" s="198"/>
+      <c r="C34" s="195"/>
+      <c r="D34" s="195"/>
+      <c r="E34" s="195"/>
+      <c r="F34" s="187" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="196" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="196" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C35" s="188">
+        <v>1.3027777777777778</v>
+      </c>
+      <c r="D35" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="187" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F35" s="187" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="197"/>
+      <c r="B36" s="197"/>
+      <c r="C36" s="199">
+        <v>0.63472222222222219</v>
+      </c>
+      <c r="D36" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="193" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F36" s="186" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="197"/>
+      <c r="B37" s="197"/>
+      <c r="C37" s="200"/>
+      <c r="D37" s="194"/>
+      <c r="E37" s="194"/>
+      <c r="F37" s="186" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="197"/>
+      <c r="B38" s="197"/>
+      <c r="C38" s="200"/>
+      <c r="D38" s="194"/>
+      <c r="E38" s="194"/>
+      <c r="F38" s="190" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="197"/>
+      <c r="B39" s="197"/>
+      <c r="C39" s="200"/>
+      <c r="D39" s="194"/>
+      <c r="E39" s="194"/>
+      <c r="F39" s="186" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="197"/>
+      <c r="B40" s="197"/>
+      <c r="C40" s="200"/>
+      <c r="D40" s="194"/>
+      <c r="E40" s="194"/>
+      <c r="F40" s="186" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="197"/>
+      <c r="B41" s="197"/>
+      <c r="C41" s="201"/>
+      <c r="D41" s="195"/>
+      <c r="E41" s="195"/>
+      <c r="F41" s="187" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="197"/>
+      <c r="B42" s="197"/>
+      <c r="C42" s="189">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="D42" s="187" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="187" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F42" s="187" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="197"/>
+      <c r="B43" s="197"/>
+      <c r="C43" s="193">
+        <v>0</v>
+      </c>
+      <c r="D43" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="193" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F43" s="186" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="197"/>
+      <c r="B44" s="197"/>
+      <c r="C44" s="194"/>
+      <c r="D44" s="194"/>
+      <c r="E44" s="194"/>
+      <c r="F44" s="186" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="198"/>
+      <c r="B45" s="198"/>
+      <c r="C45" s="195"/>
+      <c r="D45" s="195"/>
+      <c r="E45" s="195"/>
+      <c r="F45" s="187" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="A1:A8"/>
+    <mergeCell ref="B1:B8"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A23:A34"/>
+    <mergeCell ref="B23:B34"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="A35:A45"/>
+    <mergeCell ref="B35:B45"/>
+    <mergeCell ref="C36:C41"/>
+    <mergeCell ref="D36:D41"/>
+    <mergeCell ref="E36:E41"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="D43:D45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -30920,8 +31847,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D03D0EE2D2295446876114B826DEF78D" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="672737267bedf5b9e80c74c088225302">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="bbb4e383-f888-41b5-a796-2bb1d9ab62ae" xmlns:ns4="530af12c-1954-46ad-9c94-ddb07003369d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c0fbb07d547c34ba17ecd0fbb537a2c" ns1:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D03D0EE2D2295446876114B826DEF78D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dff6746d92cd1cb27242c09b947fd69b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="bbb4e383-f888-41b5-a796-2bb1d9ab62ae" xmlns:ns4="530af12c-1954-46ad-9c94-ddb07003369d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05708c9b62f10479a37610d520e71c6e" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="bbb4e383-f888-41b5-a796-2bb1d9ab62ae"/>
     <xsd:import namespace="530af12c-1954-46ad-9c94-ddb07003369d"/>
@@ -30943,6 +31870,9 @@
                 <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -31037,6 +31967,23 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="21" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="22" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -31143,16 +32090,16 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5536D9E3-D332-4E90-BF7B-48E6B0DB3F0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="bbb4e383-f888-41b5-a796-2bb1d9ab62ae"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="bbb4e383-f888-41b5-a796-2bb1d9ab62ae"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="530af12c-1954-46ad-9c94-ddb07003369d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -31166,7 +32113,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFB09BA0-4BE5-4947-B434-0DF2A857D4E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EADB11-8C90-4084-85D5-E818BD2D08C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>

</xml_diff>

<commit_message>
Add r_dprio0_tx offset 0x218 bit [31:29] phasecom fifo rd delay setting
Signed-off-by: Julie Zhang <julie.zhang@intel.com>
</commit_message>
<xml_diff>
--- a/docs/open_source_aib_csr.xlsx
+++ b/docs/open_source_aib_csr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huizhan1\open_source\aib-phy-hardware\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F4749A-A31F-40CD-A3A5-449355982B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4D11AC-1EEA-4EE6-94E9-8ED4F0E1F79A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="1950" windowWidth="23040" windowHeight="12915" activeTab="4" xr2:uid="{C6002A17-3870-4AD4-B97B-45CCDF04E806}"/>
+    <workbookView xWindow="4110" yWindow="3390" windowWidth="23040" windowHeight="12915" activeTab="4" xr2:uid="{C6002A17-3870-4AD4-B97B-45CCDF04E806}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>

</xml_diff>